<commit_message>
italicize names in missing tissues
</commit_message>
<xml_diff>
--- a/docs/suboscine_missing_tissues.xlsx
+++ b/docs/suboscine_missing_tissues.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgharvey/Dropbox/My Mac (UTFVFD57C7MNHY)/Documents/apps/GitHub/mgharvey.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EBAF4A6B-0635-0645-8D1F-3E1CE46000BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BF8026-929E-6145-8238-DED0AF2C53B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="460" windowWidth="28040" windowHeight="16480"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suboscine_missing_tissues" sheetId="1" r:id="rId1"/>
@@ -3703,8 +3703,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3848,6 +3848,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -4211,7 +4219,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4222,6 +4230,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -4577,11 +4588,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A393" workbookViewId="0">
-      <selection activeCell="B404" sqref="B404"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -4604,7 +4615,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -4615,7 +4626,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4626,7 +4637,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -4637,7 +4648,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -4648,7 +4659,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -4659,7 +4670,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -4670,7 +4681,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -4681,7 +4692,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -4692,7 +4703,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -4703,7 +4714,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -4714,7 +4725,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -4725,7 +4736,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -4736,7 +4747,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -4747,7 +4758,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -4758,7 +4769,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -4769,7 +4780,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -4780,7 +4791,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -4791,7 +4802,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -4802,7 +4813,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -4813,7 +4824,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -4824,7 +4835,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -4835,7 +4846,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -4846,7 +4857,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -4857,7 +4868,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -4868,7 +4879,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -4878,8 +4889,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A27" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -4890,7 +4901,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -4901,7 +4912,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -4912,7 +4923,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -4923,7 +4934,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -4934,7 +4945,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -4945,7 +4956,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -4956,7 +4967,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -4967,7 +4978,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -4978,7 +4989,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -4989,7 +5000,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="52" x14ac:dyDescent="0.15">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -5000,7 +5011,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -5011,7 +5022,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="5" t="s">
         <v>114</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -5022,7 +5033,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -5033,7 +5044,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -5044,7 +5055,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="5" t="s">
         <v>123</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -5055,7 +5066,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="5" t="s">
         <v>125</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -5066,7 +5077,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -5077,7 +5088,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -5088,7 +5099,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="52" x14ac:dyDescent="0.15">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="5" t="s">
         <v>134</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -5099,7 +5110,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="5" t="s">
         <v>137</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -5110,7 +5121,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="5" t="s">
         <v>139</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -5121,7 +5132,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="5" t="s">
         <v>142</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -5132,7 +5143,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="5" t="s">
         <v>145</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -5143,7 +5154,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="5" t="s">
         <v>148</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -5154,7 +5165,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="5" t="s">
         <v>151</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -5165,7 +5176,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="5" t="s">
         <v>154</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -5176,7 +5187,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="5" t="s">
         <v>157</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -5187,7 +5198,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="5" t="s">
         <v>159</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -5198,7 +5209,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -5209,7 +5220,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="5" t="s">
         <v>165</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -5220,7 +5231,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="5" t="s">
         <v>168</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -5231,7 +5242,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -5242,7 +5253,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="5" t="s">
         <v>174</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -5253,7 +5264,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="5" t="s">
         <v>177</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -5264,7 +5275,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="5" t="s">
         <v>180</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -5275,7 +5286,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="5" t="s">
         <v>183</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -5286,7 +5297,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="5" t="s">
         <v>186</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -5297,7 +5308,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="5" t="s">
         <v>189</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -5308,7 +5319,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="5" t="s">
         <v>192</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -5319,7 +5330,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="5" t="s">
         <v>195</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -5330,7 +5341,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="5" t="s">
         <v>198</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -5341,7 +5352,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="5" t="s">
         <v>201</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -5352,7 +5363,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="5" t="s">
         <v>204</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -5363,7 +5374,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -5374,7 +5385,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="5" t="s">
         <v>210</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -5385,7 +5396,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="5" t="s">
         <v>213</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -5396,7 +5407,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="5" t="s">
         <v>216</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -5407,7 +5418,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="5" t="s">
         <v>219</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -5418,7 +5429,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="5" t="s">
         <v>222</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -5429,7 +5440,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="5" t="s">
         <v>225</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -5439,8 +5450,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A78" s="3" t="s">
+    <row r="78" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A78" s="5" t="s">
         <v>228</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -5451,7 +5462,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="5" t="s">
         <v>231</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -5462,7 +5473,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="5" t="s">
         <v>234</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -5473,7 +5484,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="5" t="s">
         <v>237</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -5484,7 +5495,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="5" t="s">
         <v>240</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -5495,7 +5506,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="5" t="s">
         <v>243</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -5506,7 +5517,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="5" t="s">
         <v>246</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -5517,7 +5528,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="5" t="s">
         <v>249</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -5528,7 +5539,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="5" t="s">
         <v>252</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -5539,7 +5550,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="5" t="s">
         <v>255</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -5550,7 +5561,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="5" t="s">
         <v>258</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -5561,7 +5572,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="5" t="s">
         <v>261</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -5572,7 +5583,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="5" t="s">
         <v>264</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -5583,7 +5594,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="5" t="s">
         <v>267</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -5594,7 +5605,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="5" t="s">
         <v>270</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -5605,7 +5616,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="5" t="s">
         <v>273</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -5616,7 +5627,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="5" t="s">
         <v>276</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -5627,7 +5638,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="5" t="s">
         <v>279</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -5638,7 +5649,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="5" t="s">
         <v>282</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -5649,7 +5660,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="5" t="s">
         <v>285</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -5660,7 +5671,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="5" t="s">
         <v>288</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -5671,7 +5682,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="5" t="s">
         <v>291</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -5682,7 +5693,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="5" t="s">
         <v>294</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -5693,7 +5704,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -5704,7 +5715,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="5" t="s">
         <v>300</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -5715,7 +5726,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="5" t="s">
         <v>303</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -5726,7 +5737,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="5" t="s">
         <v>306</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -5737,7 +5748,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="5" t="s">
         <v>309</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -5748,7 +5759,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="5" t="s">
         <v>312</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -5759,7 +5770,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="5" t="s">
         <v>315</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -5770,7 +5781,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="5" t="s">
         <v>318</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -5781,7 +5792,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="5" t="s">
         <v>321</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -5792,7 +5803,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="5" t="s">
         <v>324</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -5803,7 +5814,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="5" t="s">
         <v>327</v>
       </c>
       <c r="B111" s="3" t="s">
@@ -5814,7 +5825,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="5" t="s">
         <v>330</v>
       </c>
       <c r="B112" s="3" t="s">
@@ -5825,7 +5836,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="5" t="s">
         <v>333</v>
       </c>
       <c r="B113" s="3" t="s">
@@ -5836,7 +5847,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="5" t="s">
         <v>336</v>
       </c>
       <c r="B114" s="3" t="s">
@@ -5847,7 +5858,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="5" t="s">
         <v>339</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -5858,7 +5869,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="65" x14ac:dyDescent="0.15">
-      <c r="A116" s="3" t="s">
+      <c r="A116" s="5" t="s">
         <v>342</v>
       </c>
       <c r="B116" s="3" t="s">
@@ -5869,7 +5880,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="5" t="s">
         <v>345</v>
       </c>
       <c r="B117" s="3" t="s">
@@ -5880,7 +5891,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="5" t="s">
         <v>348</v>
       </c>
       <c r="B118" s="3" t="s">
@@ -5891,7 +5902,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="5" t="s">
         <v>351</v>
       </c>
       <c r="B119" s="3" t="s">
@@ -5902,7 +5913,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="5" t="s">
         <v>354</v>
       </c>
       <c r="B120" s="3" t="s">
@@ -5913,7 +5924,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A121" s="3" t="s">
+      <c r="A121" s="5" t="s">
         <v>357</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -5924,7 +5935,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A122" s="3" t="s">
+      <c r="A122" s="5" t="s">
         <v>360</v>
       </c>
       <c r="B122" s="3" t="s">
@@ -5935,7 +5946,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="5" t="s">
         <v>362</v>
       </c>
       <c r="B123" s="3" t="s">
@@ -5946,7 +5957,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="5" t="s">
         <v>365</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -5957,7 +5968,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A125" s="3" t="s">
+      <c r="A125" s="5" t="s">
         <v>367</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -5968,7 +5979,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A126" s="3" t="s">
+      <c r="A126" s="5" t="s">
         <v>370</v>
       </c>
       <c r="B126" s="3" t="s">
@@ -5979,7 +5990,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="5" t="s">
         <v>373</v>
       </c>
       <c r="B127" s="3" t="s">
@@ -5990,7 +6001,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="5" t="s">
         <v>376</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -6001,7 +6012,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A129" s="3" t="s">
+      <c r="A129" s="5" t="s">
         <v>378</v>
       </c>
       <c r="B129" s="3" t="s">
@@ -6012,7 +6023,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A130" s="3" t="s">
+      <c r="A130" s="5" t="s">
         <v>380</v>
       </c>
       <c r="B130" s="3" t="s">
@@ -6023,7 +6034,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="5" t="s">
         <v>383</v>
       </c>
       <c r="B131" s="3" t="s">
@@ -6034,7 +6045,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A132" s="3" t="s">
+      <c r="A132" s="5" t="s">
         <v>386</v>
       </c>
       <c r="B132" s="3" t="s">
@@ -6045,7 +6056,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="78" x14ac:dyDescent="0.15">
-      <c r="A133" s="3" t="s">
+      <c r="A133" s="5" t="s">
         <v>389</v>
       </c>
       <c r="B133" s="3" t="s">
@@ -6056,7 +6067,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="65" x14ac:dyDescent="0.15">
-      <c r="A134" s="3" t="s">
+      <c r="A134" s="5" t="s">
         <v>392</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -6067,7 +6078,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="52" x14ac:dyDescent="0.15">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="5" t="s">
         <v>395</v>
       </c>
       <c r="B135" s="3" t="s">
@@ -6078,7 +6089,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A136" s="3" t="s">
+      <c r="A136" s="5" t="s">
         <v>398</v>
       </c>
       <c r="B136" s="3" t="s">
@@ -6089,7 +6100,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="5" t="s">
         <v>401</v>
       </c>
       <c r="B137" s="3" t="s">
@@ -6100,7 +6111,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A138" s="3" t="s">
+      <c r="A138" s="5" t="s">
         <v>404</v>
       </c>
       <c r="B138" s="3" t="s">
@@ -6111,7 +6122,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A139" s="3" t="s">
+      <c r="A139" s="5" t="s">
         <v>407</v>
       </c>
       <c r="B139" s="3" t="s">
@@ -6122,7 +6133,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A140" s="3" t="s">
+      <c r="A140" s="5" t="s">
         <v>410</v>
       </c>
       <c r="B140" s="3" t="s">
@@ -6133,7 +6144,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A141" s="3" t="s">
+      <c r="A141" s="5" t="s">
         <v>413</v>
       </c>
       <c r="B141" s="3" t="s">
@@ -6144,7 +6155,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A142" s="3" t="s">
+      <c r="A142" s="5" t="s">
         <v>416</v>
       </c>
       <c r="B142" s="3" t="s">
@@ -6155,7 +6166,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A143" s="3" t="s">
+      <c r="A143" s="5" t="s">
         <v>419</v>
       </c>
       <c r="B143" s="3" t="s">
@@ -6166,7 +6177,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="5" t="s">
         <v>422</v>
       </c>
       <c r="B144" s="3" t="s">
@@ -6177,7 +6188,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="5" t="s">
         <v>425</v>
       </c>
       <c r="B145" s="3" t="s">
@@ -6188,7 +6199,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="5" t="s">
         <v>428</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -6199,7 +6210,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="5" t="s">
         <v>431</v>
       </c>
       <c r="B147" s="3" t="s">
@@ -6210,7 +6221,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A148" s="3" t="s">
+      <c r="A148" s="5" t="s">
         <v>434</v>
       </c>
       <c r="B148" s="3" t="s">
@@ -6221,7 +6232,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A149" s="3" t="s">
+      <c r="A149" s="5" t="s">
         <v>437</v>
       </c>
       <c r="B149" s="3" t="s">
@@ -6232,7 +6243,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A150" s="3" t="s">
+      <c r="A150" s="5" t="s">
         <v>440</v>
       </c>
       <c r="B150" s="3" t="s">
@@ -6243,7 +6254,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A151" s="3" t="s">
+      <c r="A151" s="5" t="s">
         <v>443</v>
       </c>
       <c r="B151" s="3" t="s">
@@ -6254,7 +6265,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A152" s="3" t="s">
+      <c r="A152" s="5" t="s">
         <v>446</v>
       </c>
       <c r="B152" s="3" t="s">
@@ -6265,7 +6276,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A153" s="3" t="s">
+      <c r="A153" s="5" t="s">
         <v>449</v>
       </c>
       <c r="B153" s="3" t="s">
@@ -6276,7 +6287,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A154" s="3" t="s">
+      <c r="A154" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B154" s="3" t="s">
@@ -6287,7 +6298,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A155" s="3" t="s">
+      <c r="A155" s="5" t="s">
         <v>455</v>
       </c>
       <c r="B155" s="3" t="s">
@@ -6298,7 +6309,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A156" s="3" t="s">
+      <c r="A156" s="5" t="s">
         <v>458</v>
       </c>
       <c r="B156" s="3" t="s">
@@ -6309,7 +6320,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A157" s="3" t="s">
+      <c r="A157" s="5" t="s">
         <v>461</v>
       </c>
       <c r="B157" s="3" t="s">
@@ -6320,7 +6331,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="5" t="s">
         <v>463</v>
       </c>
       <c r="B158" s="3" t="s">
@@ -6331,7 +6342,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="5" t="s">
         <v>466</v>
       </c>
       <c r="B159" s="3" t="s">
@@ -6342,7 +6353,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="5" t="s">
         <v>469</v>
       </c>
       <c r="B160" s="3" t="s">
@@ -6353,7 +6364,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="5" t="s">
         <v>472</v>
       </c>
       <c r="B161" s="3" t="s">
@@ -6364,7 +6375,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="5" t="s">
         <v>475</v>
       </c>
       <c r="B162" s="3" t="s">
@@ -6375,7 +6386,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="5" t="s">
         <v>478</v>
       </c>
       <c r="B163" s="3" t="s">
@@ -6386,7 +6397,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="5" t="s">
         <v>481</v>
       </c>
       <c r="B164" s="3" t="s">
@@ -6397,7 +6408,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="5" t="s">
         <v>484</v>
       </c>
       <c r="B165" s="3" t="s">
@@ -6408,7 +6419,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A166" s="3" t="s">
+      <c r="A166" s="5" t="s">
         <v>487</v>
       </c>
       <c r="B166" s="3" t="s">
@@ -6419,7 +6430,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A167" s="3" t="s">
+      <c r="A167" s="5" t="s">
         <v>490</v>
       </c>
       <c r="B167" s="3" t="s">
@@ -6430,7 +6441,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="5" t="s">
         <v>493</v>
       </c>
       <c r="B168" s="3" t="s">
@@ -6441,7 +6452,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A169" s="3" t="s">
+      <c r="A169" s="5" t="s">
         <v>496</v>
       </c>
       <c r="B169" s="3" t="s">
@@ -6452,7 +6463,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A170" s="3" t="s">
+      <c r="A170" s="5" t="s">
         <v>499</v>
       </c>
       <c r="B170" s="3" t="s">
@@ -6463,7 +6474,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A171" s="3" t="s">
+      <c r="A171" s="5" t="s">
         <v>502</v>
       </c>
       <c r="B171" s="3" t="s">
@@ -6474,7 +6485,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A172" s="3" t="s">
+      <c r="A172" s="5" t="s">
         <v>505</v>
       </c>
       <c r="B172" s="3" t="s">
@@ -6485,7 +6496,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A173" s="3" t="s">
+      <c r="A173" s="5" t="s">
         <v>508</v>
       </c>
       <c r="B173" s="3" t="s">
@@ -6496,7 +6507,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A174" s="3" t="s">
+      <c r="A174" s="5" t="s">
         <v>511</v>
       </c>
       <c r="B174" s="3" t="s">
@@ -6507,7 +6518,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A175" s="3" t="s">
+      <c r="A175" s="5" t="s">
         <v>514</v>
       </c>
       <c r="B175" s="3" t="s">
@@ -6518,7 +6529,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A176" s="3" t="s">
+      <c r="A176" s="5" t="s">
         <v>517</v>
       </c>
       <c r="B176" s="3" t="s">
@@ -6529,7 +6540,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A177" s="3" t="s">
+      <c r="A177" s="5" t="s">
         <v>520</v>
       </c>
       <c r="B177" s="3" t="s">
@@ -6540,7 +6551,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A178" s="3" t="s">
+      <c r="A178" s="5" t="s">
         <v>523</v>
       </c>
       <c r="B178" s="3" t="s">
@@ -6550,8 +6561,8 @@
         <v>525</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A179" s="3" t="s">
+    <row r="179" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A179" s="5" t="s">
         <v>526</v>
       </c>
       <c r="B179" s="3" t="s">
@@ -6562,7 +6573,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A180" s="3" t="s">
+      <c r="A180" s="5" t="s">
         <v>529</v>
       </c>
       <c r="B180" s="3" t="s">
@@ -6573,7 +6584,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A181" s="3" t="s">
+      <c r="A181" s="5" t="s">
         <v>532</v>
       </c>
       <c r="B181" s="3" t="s">
@@ -6584,7 +6595,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A182" s="3" t="s">
+      <c r="A182" s="5" t="s">
         <v>535</v>
       </c>
       <c r="B182" s="3" t="s">
@@ -6595,7 +6606,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="5" t="s">
         <v>538</v>
       </c>
       <c r="B183" s="3" t="s">
@@ -6606,7 +6617,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A184" s="3" t="s">
+      <c r="A184" s="5" t="s">
         <v>541</v>
       </c>
       <c r="B184" s="3" t="s">
@@ -6617,7 +6628,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A185" s="3" t="s">
+      <c r="A185" s="5" t="s">
         <v>544</v>
       </c>
       <c r="B185" s="3" t="s">
@@ -6628,7 +6639,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A186" s="3" t="s">
+      <c r="A186" s="5" t="s">
         <v>547</v>
       </c>
       <c r="B186" s="3" t="s">
@@ -6639,7 +6650,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A187" s="3" t="s">
+      <c r="A187" s="5" t="s">
         <v>550</v>
       </c>
       <c r="B187" s="3" t="s">
@@ -6650,7 +6661,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A188" s="3" t="s">
+      <c r="A188" s="5" t="s">
         <v>553</v>
       </c>
       <c r="B188" s="3" t="s">
@@ -6661,7 +6672,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A189" s="3" t="s">
+      <c r="A189" s="5" t="s">
         <v>556</v>
       </c>
       <c r="B189" s="3" t="s">
@@ -6672,7 +6683,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A190" s="3" t="s">
+      <c r="A190" s="5" t="s">
         <v>559</v>
       </c>
       <c r="B190" s="3" t="s">
@@ -6683,7 +6694,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A191" s="3" t="s">
+      <c r="A191" s="5" t="s">
         <v>562</v>
       </c>
       <c r="B191" s="3" t="s">
@@ -6694,7 +6705,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A192" s="3" t="s">
+      <c r="A192" s="5" t="s">
         <v>565</v>
       </c>
       <c r="B192" s="3" t="s">
@@ -6705,7 +6716,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A193" s="3" t="s">
+      <c r="A193" s="5" t="s">
         <v>567</v>
       </c>
       <c r="B193" s="3" t="s">
@@ -6716,7 +6727,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A194" s="3" t="s">
+      <c r="A194" s="5" t="s">
         <v>570</v>
       </c>
       <c r="B194" s="3" t="s">
@@ -6727,7 +6738,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A195" s="3" t="s">
+      <c r="A195" s="5" t="s">
         <v>573</v>
       </c>
       <c r="B195" s="3" t="s">
@@ -6738,7 +6749,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A196" s="3" t="s">
+      <c r="A196" s="5" t="s">
         <v>576</v>
       </c>
       <c r="B196" s="3" t="s">
@@ -6749,7 +6760,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A197" s="3" t="s">
+      <c r="A197" s="5" t="s">
         <v>579</v>
       </c>
       <c r="B197" s="3" t="s">
@@ -6760,7 +6771,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A198" s="3" t="s">
+      <c r="A198" s="5" t="s">
         <v>582</v>
       </c>
       <c r="B198" s="3" t="s">
@@ -6771,7 +6782,7 @@
       </c>
     </row>
     <row r="199" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A199" s="3" t="s">
+      <c r="A199" s="5" t="s">
         <v>585</v>
       </c>
       <c r="B199" s="3" t="s">
@@ -6782,7 +6793,7 @@
       </c>
     </row>
     <row r="200" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A200" s="3" t="s">
+      <c r="A200" s="5" t="s">
         <v>587</v>
       </c>
       <c r="B200" s="3" t="s">
@@ -6793,7 +6804,7 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A201" s="3" t="s">
+      <c r="A201" s="5" t="s">
         <v>590</v>
       </c>
       <c r="B201" s="3" t="s">
@@ -6804,7 +6815,7 @@
       </c>
     </row>
     <row r="202" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A202" s="3" t="s">
+      <c r="A202" s="5" t="s">
         <v>593</v>
       </c>
       <c r="B202" s="3" t="s">
@@ -6815,7 +6826,7 @@
       </c>
     </row>
     <row r="203" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A203" s="3" t="s">
+      <c r="A203" s="5" t="s">
         <v>595</v>
       </c>
       <c r="B203" s="3" t="s">
@@ -6826,7 +6837,7 @@
       </c>
     </row>
     <row r="204" spans="1:3" ht="52" x14ac:dyDescent="0.15">
-      <c r="A204" s="3" t="s">
+      <c r="A204" s="5" t="s">
         <v>598</v>
       </c>
       <c r="B204" s="3" t="s">
@@ -6837,7 +6848,7 @@
       </c>
     </row>
     <row r="205" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A205" s="3" t="s">
+      <c r="A205" s="5" t="s">
         <v>601</v>
       </c>
       <c r="B205" s="3" t="s">
@@ -6848,7 +6859,7 @@
       </c>
     </row>
     <row r="206" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A206" s="3" t="s">
+      <c r="A206" s="5" t="s">
         <v>604</v>
       </c>
       <c r="B206" s="3" t="s">
@@ -6859,7 +6870,7 @@
       </c>
     </row>
     <row r="207" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A207" s="3" t="s">
+      <c r="A207" s="5" t="s">
         <v>607</v>
       </c>
       <c r="B207" s="3" t="s">
@@ -6870,7 +6881,7 @@
       </c>
     </row>
     <row r="208" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A208" s="3" t="s">
+      <c r="A208" s="5" t="s">
         <v>610</v>
       </c>
       <c r="B208" s="3" t="s">
@@ -6881,7 +6892,7 @@
       </c>
     </row>
     <row r="209" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A209" s="3" t="s">
+      <c r="A209" s="5" t="s">
         <v>613</v>
       </c>
       <c r="B209" s="3" t="s">
@@ -6892,7 +6903,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A210" s="3" t="s">
+      <c r="A210" s="5" t="s">
         <v>616</v>
       </c>
       <c r="B210" s="3" t="s">
@@ -6903,7 +6914,7 @@
       </c>
     </row>
     <row r="211" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A211" s="3" t="s">
+      <c r="A211" s="5" t="s">
         <v>619</v>
       </c>
       <c r="B211" s="3" t="s">
@@ -6914,7 +6925,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A212" s="3" t="s">
+      <c r="A212" s="5" t="s">
         <v>622</v>
       </c>
       <c r="B212" s="3" t="s">
@@ -6925,7 +6936,7 @@
       </c>
     </row>
     <row r="213" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A213" s="3" t="s">
+      <c r="A213" s="5" t="s">
         <v>625</v>
       </c>
       <c r="B213" s="3" t="s">
@@ -6936,7 +6947,7 @@
       </c>
     </row>
     <row r="214" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A214" s="3" t="s">
+      <c r="A214" s="5" t="s">
         <v>628</v>
       </c>
       <c r="B214" s="3" t="s">
@@ -6947,7 +6958,7 @@
       </c>
     </row>
     <row r="215" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A215" s="3" t="s">
+      <c r="A215" s="5" t="s">
         <v>631</v>
       </c>
       <c r="B215" s="3" t="s">
@@ -6958,7 +6969,7 @@
       </c>
     </row>
     <row r="216" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A216" s="3" t="s">
+      <c r="A216" s="5" t="s">
         <v>634</v>
       </c>
       <c r="B216" s="3" t="s">
@@ -6969,7 +6980,7 @@
       </c>
     </row>
     <row r="217" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A217" s="3" t="s">
+      <c r="A217" s="5" t="s">
         <v>637</v>
       </c>
       <c r="B217" s="3" t="s">
@@ -6980,7 +6991,7 @@
       </c>
     </row>
     <row r="218" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A218" s="3" t="s">
+      <c r="A218" s="5" t="s">
         <v>640</v>
       </c>
       <c r="B218" s="3" t="s">
@@ -6991,7 +7002,7 @@
       </c>
     </row>
     <row r="219" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A219" s="3" t="s">
+      <c r="A219" s="5" t="s">
         <v>643</v>
       </c>
       <c r="B219" s="3" t="s">
@@ -7002,7 +7013,7 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A220" s="3" t="s">
+      <c r="A220" s="5" t="s">
         <v>646</v>
       </c>
       <c r="B220" s="3" t="s">
@@ -7013,7 +7024,7 @@
       </c>
     </row>
     <row r="221" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A221" s="3" t="s">
+      <c r="A221" s="5" t="s">
         <v>649</v>
       </c>
       <c r="B221" s="3" t="s">
@@ -7024,7 +7035,7 @@
       </c>
     </row>
     <row r="222" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A222" s="3" t="s">
+      <c r="A222" s="5" t="s">
         <v>652</v>
       </c>
       <c r="B222" s="3" t="s">
@@ -7035,7 +7046,7 @@
       </c>
     </row>
     <row r="223" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A223" s="3" t="s">
+      <c r="A223" s="5" t="s">
         <v>655</v>
       </c>
       <c r="B223" s="3" t="s">
@@ -7046,7 +7057,7 @@
       </c>
     </row>
     <row r="224" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A224" s="3" t="s">
+      <c r="A224" s="5" t="s">
         <v>657</v>
       </c>
       <c r="B224" s="3" t="s">
@@ -7057,7 +7068,7 @@
       </c>
     </row>
     <row r="225" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A225" s="3" t="s">
+      <c r="A225" s="5" t="s">
         <v>660</v>
       </c>
       <c r="B225" s="3" t="s">
@@ -7068,7 +7079,7 @@
       </c>
     </row>
     <row r="226" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A226" s="3" t="s">
+      <c r="A226" s="5" t="s">
         <v>663</v>
       </c>
       <c r="B226" s="3" t="s">
@@ -7079,7 +7090,7 @@
       </c>
     </row>
     <row r="227" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A227" s="3" t="s">
+      <c r="A227" s="5" t="s">
         <v>666</v>
       </c>
       <c r="B227" s="3" t="s">
@@ -7090,7 +7101,7 @@
       </c>
     </row>
     <row r="228" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A228" s="3" t="s">
+      <c r="A228" s="5" t="s">
         <v>669</v>
       </c>
       <c r="B228" s="3" t="s">
@@ -7101,7 +7112,7 @@
       </c>
     </row>
     <row r="229" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A229" s="3" t="s">
+      <c r="A229" s="5" t="s">
         <v>671</v>
       </c>
       <c r="B229" s="3" t="s">
@@ -7112,7 +7123,7 @@
       </c>
     </row>
     <row r="230" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A230" s="3" t="s">
+      <c r="A230" s="5" t="s">
         <v>674</v>
       </c>
       <c r="B230" s="3" t="s">
@@ -7123,7 +7134,7 @@
       </c>
     </row>
     <row r="231" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A231" s="3" t="s">
+      <c r="A231" s="5" t="s">
         <v>677</v>
       </c>
       <c r="B231" s="3" t="s">
@@ -7134,7 +7145,7 @@
       </c>
     </row>
     <row r="232" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A232" s="3" t="s">
+      <c r="A232" s="5" t="s">
         <v>680</v>
       </c>
       <c r="B232" s="3" t="s">
@@ -7145,7 +7156,7 @@
       </c>
     </row>
     <row r="233" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A233" s="3" t="s">
+      <c r="A233" s="5" t="s">
         <v>682</v>
       </c>
       <c r="B233" s="3" t="s">
@@ -7156,7 +7167,7 @@
       </c>
     </row>
     <row r="234" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A234" s="3" t="s">
+      <c r="A234" s="5" t="s">
         <v>685</v>
       </c>
       <c r="B234" s="3" t="s">
@@ -7167,7 +7178,7 @@
       </c>
     </row>
     <row r="235" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A235" s="3" t="s">
+      <c r="A235" s="5" t="s">
         <v>688</v>
       </c>
       <c r="B235" s="3" t="s">
@@ -7178,7 +7189,7 @@
       </c>
     </row>
     <row r="236" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A236" s="3" t="s">
+      <c r="A236" s="5" t="s">
         <v>690</v>
       </c>
       <c r="B236" s="3" t="s">
@@ -7189,7 +7200,7 @@
       </c>
     </row>
     <row r="237" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A237" s="3" t="s">
+      <c r="A237" s="5" t="s">
         <v>692</v>
       </c>
       <c r="B237" s="3" t="s">
@@ -7200,7 +7211,7 @@
       </c>
     </row>
     <row r="238" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A238" s="3" t="s">
+      <c r="A238" s="5" t="s">
         <v>694</v>
       </c>
       <c r="B238" s="3" t="s">
@@ -7211,7 +7222,7 @@
       </c>
     </row>
     <row r="239" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A239" s="3" t="s">
+      <c r="A239" s="5" t="s">
         <v>697</v>
       </c>
       <c r="B239" s="3" t="s">
@@ -7222,7 +7233,7 @@
       </c>
     </row>
     <row r="240" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A240" s="3" t="s">
+      <c r="A240" s="5" t="s">
         <v>700</v>
       </c>
       <c r="B240" s="3" t="s">
@@ -7233,7 +7244,7 @@
       </c>
     </row>
     <row r="241" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A241" s="3" t="s">
+      <c r="A241" s="5" t="s">
         <v>702</v>
       </c>
       <c r="B241" s="3" t="s">
@@ -7244,7 +7255,7 @@
       </c>
     </row>
     <row r="242" spans="1:3" ht="52" x14ac:dyDescent="0.15">
-      <c r="A242" s="3" t="s">
+      <c r="A242" s="5" t="s">
         <v>705</v>
       </c>
       <c r="B242" s="3" t="s">
@@ -7255,7 +7266,7 @@
       </c>
     </row>
     <row r="243" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A243" s="3" t="s">
+      <c r="A243" s="5" t="s">
         <v>707</v>
       </c>
       <c r="B243" s="3" t="s">
@@ -7266,7 +7277,7 @@
       </c>
     </row>
     <row r="244" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A244" s="3" t="s">
+      <c r="A244" s="5" t="s">
         <v>710</v>
       </c>
       <c r="B244" s="3" t="s">
@@ -7277,7 +7288,7 @@
       </c>
     </row>
     <row r="245" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A245" s="3" t="s">
+      <c r="A245" s="5" t="s">
         <v>713</v>
       </c>
       <c r="B245" s="3" t="s">
@@ -7288,7 +7299,7 @@
       </c>
     </row>
     <row r="246" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A246" s="3" t="s">
+      <c r="A246" s="5" t="s">
         <v>716</v>
       </c>
       <c r="B246" s="3" t="s">
@@ -7299,7 +7310,7 @@
       </c>
     </row>
     <row r="247" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A247" s="3" t="s">
+      <c r="A247" s="5" t="s">
         <v>719</v>
       </c>
       <c r="B247" s="3" t="s">
@@ -7310,7 +7321,7 @@
       </c>
     </row>
     <row r="248" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A248" s="3" t="s">
+      <c r="A248" s="5" t="s">
         <v>722</v>
       </c>
       <c r="B248" s="3" t="s">
@@ -7321,7 +7332,7 @@
       </c>
     </row>
     <row r="249" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A249" s="3" t="s">
+      <c r="A249" s="5" t="s">
         <v>725</v>
       </c>
       <c r="B249" s="3" t="s">
@@ -7332,7 +7343,7 @@
       </c>
     </row>
     <row r="250" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A250" s="3" t="s">
+      <c r="A250" s="5" t="s">
         <v>728</v>
       </c>
       <c r="B250" s="3" t="s">
@@ -7343,7 +7354,7 @@
       </c>
     </row>
     <row r="251" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A251" s="3" t="s">
+      <c r="A251" s="5" t="s">
         <v>731</v>
       </c>
       <c r="B251" s="3" t="s">
@@ -7354,7 +7365,7 @@
       </c>
     </row>
     <row r="252" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A252" s="3" t="s">
+      <c r="A252" s="5" t="s">
         <v>734</v>
       </c>
       <c r="B252" s="3" t="s">
@@ -7365,7 +7376,7 @@
       </c>
     </row>
     <row r="253" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A253" s="3" t="s">
+      <c r="A253" s="5" t="s">
         <v>737</v>
       </c>
       <c r="B253" s="3" t="s">
@@ -7376,7 +7387,7 @@
       </c>
     </row>
     <row r="254" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A254" s="3" t="s">
+      <c r="A254" s="5" t="s">
         <v>740</v>
       </c>
       <c r="B254" s="3" t="s">
@@ -7387,7 +7398,7 @@
       </c>
     </row>
     <row r="255" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A255" s="3" t="s">
+      <c r="A255" s="5" t="s">
         <v>743</v>
       </c>
       <c r="B255" s="3" t="s">
@@ -7398,7 +7409,7 @@
       </c>
     </row>
     <row r="256" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A256" s="3" t="s">
+      <c r="A256" s="5" t="s">
         <v>746</v>
       </c>
       <c r="B256" s="3" t="s">
@@ -7409,7 +7420,7 @@
       </c>
     </row>
     <row r="257" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A257" s="3" t="s">
+      <c r="A257" s="5" t="s">
         <v>749</v>
       </c>
       <c r="B257" s="3" t="s">
@@ -7420,7 +7431,7 @@
       </c>
     </row>
     <row r="258" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A258" s="3" t="s">
+      <c r="A258" s="5" t="s">
         <v>752</v>
       </c>
       <c r="B258" s="3" t="s">
@@ -7431,7 +7442,7 @@
       </c>
     </row>
     <row r="259" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A259" s="3" t="s">
+      <c r="A259" s="5" t="s">
         <v>755</v>
       </c>
       <c r="B259" s="3" t="s">
@@ -7442,7 +7453,7 @@
       </c>
     </row>
     <row r="260" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A260" s="3" t="s">
+      <c r="A260" s="5" t="s">
         <v>757</v>
       </c>
       <c r="B260" s="3" t="s">
@@ -7453,7 +7464,7 @@
       </c>
     </row>
     <row r="261" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A261" s="3" t="s">
+      <c r="A261" s="5" t="s">
         <v>758</v>
       </c>
       <c r="B261" s="3" t="s">
@@ -7464,7 +7475,7 @@
       </c>
     </row>
     <row r="262" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A262" s="3" t="s">
+      <c r="A262" s="5" t="s">
         <v>761</v>
       </c>
       <c r="B262" s="3" t="s">
@@ -7475,7 +7486,7 @@
       </c>
     </row>
     <row r="263" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A263" s="3" t="s">
+      <c r="A263" s="5" t="s">
         <v>764</v>
       </c>
       <c r="B263" s="3" t="s">
@@ -7486,7 +7497,7 @@
       </c>
     </row>
     <row r="264" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A264" s="3" t="s">
+      <c r="A264" s="5" t="s">
         <v>767</v>
       </c>
       <c r="B264" s="3" t="s">
@@ -7497,7 +7508,7 @@
       </c>
     </row>
     <row r="265" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A265" s="3" t="s">
+      <c r="A265" s="5" t="s">
         <v>769</v>
       </c>
       <c r="B265" s="3" t="s">
@@ -7508,7 +7519,7 @@
       </c>
     </row>
     <row r="266" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A266" s="3" t="s">
+      <c r="A266" s="5" t="s">
         <v>772</v>
       </c>
       <c r="B266" s="3" t="s">
@@ -7519,7 +7530,7 @@
       </c>
     </row>
     <row r="267" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A267" s="3" t="s">
+      <c r="A267" s="5" t="s">
         <v>775</v>
       </c>
       <c r="B267" s="3" t="s">
@@ -7530,7 +7541,7 @@
       </c>
     </row>
     <row r="268" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A268" s="3" t="s">
+      <c r="A268" s="5" t="s">
         <v>778</v>
       </c>
       <c r="B268" s="3" t="s">
@@ -7541,7 +7552,7 @@
       </c>
     </row>
     <row r="269" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A269" s="3" t="s">
+      <c r="A269" s="5" t="s">
         <v>781</v>
       </c>
       <c r="B269" s="3" t="s">
@@ -7552,7 +7563,7 @@
       </c>
     </row>
     <row r="270" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A270" s="3" t="s">
+      <c r="A270" s="5" t="s">
         <v>784</v>
       </c>
       <c r="B270" s="3" t="s">
@@ -7563,7 +7574,7 @@
       </c>
     </row>
     <row r="271" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A271" s="3" t="s">
+      <c r="A271" s="5" t="s">
         <v>787</v>
       </c>
       <c r="B271" s="3" t="s">
@@ -7574,7 +7585,7 @@
       </c>
     </row>
     <row r="272" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A272" s="3" t="s">
+      <c r="A272" s="5" t="s">
         <v>790</v>
       </c>
       <c r="B272" s="3" t="s">
@@ -7585,7 +7596,7 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A273" s="3" t="s">
+      <c r="A273" s="5" t="s">
         <v>793</v>
       </c>
       <c r="B273" s="3" t="s">
@@ -7596,7 +7607,7 @@
       </c>
     </row>
     <row r="274" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A274" s="3" t="s">
+      <c r="A274" s="5" t="s">
         <v>796</v>
       </c>
       <c r="B274" s="3" t="s">
@@ -7607,7 +7618,7 @@
       </c>
     </row>
     <row r="275" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A275" s="3" t="s">
+      <c r="A275" s="5" t="s">
         <v>798</v>
       </c>
       <c r="B275" s="3" t="s">
@@ -7618,7 +7629,7 @@
       </c>
     </row>
     <row r="276" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A276" s="3" t="s">
+      <c r="A276" s="5" t="s">
         <v>801</v>
       </c>
       <c r="B276" s="3" t="s">
@@ -7629,7 +7640,7 @@
       </c>
     </row>
     <row r="277" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A277" s="3" t="s">
+      <c r="A277" s="5" t="s">
         <v>804</v>
       </c>
       <c r="B277" s="3" t="s">
@@ -7640,7 +7651,7 @@
       </c>
     </row>
     <row r="278" spans="1:3" ht="65" x14ac:dyDescent="0.15">
-      <c r="A278" s="3" t="s">
+      <c r="A278" s="5" t="s">
         <v>807</v>
       </c>
       <c r="B278" s="3" t="s">
@@ -7651,7 +7662,7 @@
       </c>
     </row>
     <row r="279" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A279" s="3" t="s">
+      <c r="A279" s="5" t="s">
         <v>810</v>
       </c>
       <c r="B279" s="3" t="s">
@@ -7662,7 +7673,7 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A280" s="3" t="s">
+      <c r="A280" s="5" t="s">
         <v>813</v>
       </c>
       <c r="B280" s="3" t="s">
@@ -7673,7 +7684,7 @@
       </c>
     </row>
     <row r="281" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A281" s="3" t="s">
+      <c r="A281" s="5" t="s">
         <v>816</v>
       </c>
       <c r="B281" s="3" t="s">
@@ -7684,7 +7695,7 @@
       </c>
     </row>
     <row r="282" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A282" s="3" t="s">
+      <c r="A282" s="5" t="s">
         <v>818</v>
       </c>
       <c r="B282" s="3" t="s">
@@ -7695,7 +7706,7 @@
       </c>
     </row>
     <row r="283" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A283" s="3" t="s">
+      <c r="A283" s="5" t="s">
         <v>821</v>
       </c>
       <c r="B283" s="3" t="s">
@@ -7706,7 +7717,7 @@
       </c>
     </row>
     <row r="284" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A284" s="3" t="s">
+      <c r="A284" s="5" t="s">
         <v>823</v>
       </c>
       <c r="B284" s="3" t="s">
@@ -7717,7 +7728,7 @@
       </c>
     </row>
     <row r="285" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A285" s="3" t="s">
+      <c r="A285" s="5" t="s">
         <v>826</v>
       </c>
       <c r="B285" s="3" t="s">
@@ -7728,7 +7739,7 @@
       </c>
     </row>
     <row r="286" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A286" s="3" t="s">
+      <c r="A286" s="5" t="s">
         <v>829</v>
       </c>
       <c r="B286" s="3" t="s">
@@ -7739,7 +7750,7 @@
       </c>
     </row>
     <row r="287" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A287" s="3" t="s">
+      <c r="A287" s="5" t="s">
         <v>832</v>
       </c>
       <c r="B287" s="3" t="s">
@@ -7750,7 +7761,7 @@
       </c>
     </row>
     <row r="288" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A288" s="3" t="s">
+      <c r="A288" s="5" t="s">
         <v>835</v>
       </c>
       <c r="B288" s="3" t="s">
@@ -7761,7 +7772,7 @@
       </c>
     </row>
     <row r="289" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A289" s="3" t="s">
+      <c r="A289" s="5" t="s">
         <v>838</v>
       </c>
       <c r="B289" s="3" t="s">
@@ -7772,7 +7783,7 @@
       </c>
     </row>
     <row r="290" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A290" s="3" t="s">
+      <c r="A290" s="5" t="s">
         <v>841</v>
       </c>
       <c r="B290" s="3" t="s">
@@ -7783,7 +7794,7 @@
       </c>
     </row>
     <row r="291" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A291" s="3" t="s">
+      <c r="A291" s="5" t="s">
         <v>844</v>
       </c>
       <c r="B291" s="3" t="s">
@@ -7794,7 +7805,7 @@
       </c>
     </row>
     <row r="292" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A292" s="3" t="s">
+      <c r="A292" s="5" t="s">
         <v>847</v>
       </c>
       <c r="B292" s="3" t="s">
@@ -7805,7 +7816,7 @@
       </c>
     </row>
     <row r="293" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A293" s="3" t="s">
+      <c r="A293" s="5" t="s">
         <v>850</v>
       </c>
       <c r="B293" s="3" t="s">
@@ -7816,7 +7827,7 @@
       </c>
     </row>
     <row r="294" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A294" s="3" t="s">
+      <c r="A294" s="5" t="s">
         <v>853</v>
       </c>
       <c r="B294" s="3" t="s">
@@ -7827,7 +7838,7 @@
       </c>
     </row>
     <row r="295" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A295" s="3" t="s">
+      <c r="A295" s="5" t="s">
         <v>856</v>
       </c>
       <c r="B295" s="3" t="s">
@@ -7838,7 +7849,7 @@
       </c>
     </row>
     <row r="296" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A296" s="3" t="s">
+      <c r="A296" s="5" t="s">
         <v>859</v>
       </c>
       <c r="B296" s="3" t="s">
@@ -7849,7 +7860,7 @@
       </c>
     </row>
     <row r="297" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A297" s="3" t="s">
+      <c r="A297" s="5" t="s">
         <v>862</v>
       </c>
       <c r="B297" s="3" t="s">
@@ -7860,7 +7871,7 @@
       </c>
     </row>
     <row r="298" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A298" s="3" t="s">
+      <c r="A298" s="5" t="s">
         <v>865</v>
       </c>
       <c r="B298" s="3" t="s">
@@ -7871,7 +7882,7 @@
       </c>
     </row>
     <row r="299" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A299" s="3" t="s">
+      <c r="A299" s="5" t="s">
         <v>868</v>
       </c>
       <c r="B299" s="3" t="s">
@@ -7882,7 +7893,7 @@
       </c>
     </row>
     <row r="300" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A300" s="3" t="s">
+      <c r="A300" s="5" t="s">
         <v>871</v>
       </c>
       <c r="B300" s="3" t="s">
@@ -7893,7 +7904,7 @@
       </c>
     </row>
     <row r="301" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A301" s="3" t="s">
+      <c r="A301" s="5" t="s">
         <v>874</v>
       </c>
       <c r="B301" s="3" t="s">
@@ -7904,7 +7915,7 @@
       </c>
     </row>
     <row r="302" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A302" s="3" t="s">
+      <c r="A302" s="5" t="s">
         <v>877</v>
       </c>
       <c r="B302" s="3" t="s">
@@ -7915,7 +7926,7 @@
       </c>
     </row>
     <row r="303" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A303" s="3" t="s">
+      <c r="A303" s="5" t="s">
         <v>879</v>
       </c>
       <c r="B303" s="3" t="s">
@@ -7926,7 +7937,7 @@
       </c>
     </row>
     <row r="304" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A304" s="3" t="s">
+      <c r="A304" s="5" t="s">
         <v>882</v>
       </c>
       <c r="B304" s="3" t="s">
@@ -7937,7 +7948,7 @@
       </c>
     </row>
     <row r="305" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A305" s="3" t="s">
+      <c r="A305" s="5" t="s">
         <v>885</v>
       </c>
       <c r="B305" s="3" t="s">
@@ -7948,7 +7959,7 @@
       </c>
     </row>
     <row r="306" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A306" s="3" t="s">
+      <c r="A306" s="5" t="s">
         <v>887</v>
       </c>
       <c r="B306" s="3" t="s">
@@ -7959,7 +7970,7 @@
       </c>
     </row>
     <row r="307" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A307" s="3" t="s">
+      <c r="A307" s="5" t="s">
         <v>889</v>
       </c>
       <c r="B307" s="3" t="s">
@@ -7970,7 +7981,7 @@
       </c>
     </row>
     <row r="308" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A308" s="3" t="s">
+      <c r="A308" s="5" t="s">
         <v>892</v>
       </c>
       <c r="B308" s="3" t="s">
@@ -7981,7 +7992,7 @@
       </c>
     </row>
     <row r="309" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A309" s="3" t="s">
+      <c r="A309" s="5" t="s">
         <v>895</v>
       </c>
       <c r="B309" s="3" t="s">
@@ -7992,7 +8003,7 @@
       </c>
     </row>
     <row r="310" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A310" s="3" t="s">
+      <c r="A310" s="5" t="s">
         <v>898</v>
       </c>
       <c r="B310" s="3" t="s">
@@ -8003,7 +8014,7 @@
       </c>
     </row>
     <row r="311" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A311" s="3" t="s">
+      <c r="A311" s="5" t="s">
         <v>901</v>
       </c>
       <c r="B311" s="3" t="s">
@@ -8014,7 +8025,7 @@
       </c>
     </row>
     <row r="312" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A312" s="3" t="s">
+      <c r="A312" s="5" t="s">
         <v>904</v>
       </c>
       <c r="B312" s="3" t="s">
@@ -8025,7 +8036,7 @@
       </c>
     </row>
     <row r="313" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A313" s="3" t="s">
+      <c r="A313" s="5" t="s">
         <v>907</v>
       </c>
       <c r="B313" s="3" t="s">
@@ -8036,7 +8047,7 @@
       </c>
     </row>
     <row r="314" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A314" s="3" t="s">
+      <c r="A314" s="5" t="s">
         <v>910</v>
       </c>
       <c r="B314" s="3" t="s">
@@ -8047,7 +8058,7 @@
       </c>
     </row>
     <row r="315" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A315" s="3" t="s">
+      <c r="A315" s="5" t="s">
         <v>913</v>
       </c>
       <c r="B315" s="3" t="s">
@@ -8058,7 +8069,7 @@
       </c>
     </row>
     <row r="316" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A316" s="3" t="s">
+      <c r="A316" s="5" t="s">
         <v>916</v>
       </c>
       <c r="B316" s="3" t="s">
@@ -8069,7 +8080,7 @@
       </c>
     </row>
     <row r="317" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A317" s="3" t="s">
+      <c r="A317" s="5" t="s">
         <v>919</v>
       </c>
       <c r="B317" s="3" t="s">
@@ -8080,7 +8091,7 @@
       </c>
     </row>
     <row r="318" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A318" s="3" t="s">
+      <c r="A318" s="5" t="s">
         <v>922</v>
       </c>
       <c r="B318" s="3" t="s">
@@ -8091,7 +8102,7 @@
       </c>
     </row>
     <row r="319" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A319" s="3" t="s">
+      <c r="A319" s="5" t="s">
         <v>924</v>
       </c>
       <c r="B319" s="3" t="s">
@@ -8102,7 +8113,7 @@
       </c>
     </row>
     <row r="320" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A320" s="3" t="s">
+      <c r="A320" s="5" t="s">
         <v>927</v>
       </c>
       <c r="B320" s="3" t="s">
@@ -8113,7 +8124,7 @@
       </c>
     </row>
     <row r="321" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A321" s="3" t="s">
+      <c r="A321" s="5" t="s">
         <v>929</v>
       </c>
       <c r="B321" s="3" t="s">
@@ -8124,7 +8135,7 @@
       </c>
     </row>
     <row r="322" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A322" s="3" t="s">
+      <c r="A322" s="5" t="s">
         <v>932</v>
       </c>
       <c r="B322" s="3" t="s">
@@ -8135,7 +8146,7 @@
       </c>
     </row>
     <row r="323" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A323" s="3" t="s">
+      <c r="A323" s="5" t="s">
         <v>934</v>
       </c>
       <c r="B323" s="3" t="s">
@@ -8146,7 +8157,7 @@
       </c>
     </row>
     <row r="324" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A324" s="3" t="s">
+      <c r="A324" s="5" t="s">
         <v>937</v>
       </c>
       <c r="B324" s="3" t="s">
@@ -8157,7 +8168,7 @@
       </c>
     </row>
     <row r="325" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A325" s="3" t="s">
+      <c r="A325" s="5" t="s">
         <v>940</v>
       </c>
       <c r="B325" s="3" t="s">
@@ -8168,7 +8179,7 @@
       </c>
     </row>
     <row r="326" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A326" s="3" t="s">
+      <c r="A326" s="5" t="s">
         <v>943</v>
       </c>
       <c r="B326" s="3" t="s">
@@ -8179,7 +8190,7 @@
       </c>
     </row>
     <row r="327" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A327" s="3" t="s">
+      <c r="A327" s="5" t="s">
         <v>946</v>
       </c>
       <c r="B327" s="3" t="s">
@@ -8190,7 +8201,7 @@
       </c>
     </row>
     <row r="328" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A328" s="3" t="s">
+      <c r="A328" s="5" t="s">
         <v>949</v>
       </c>
       <c r="B328" s="3" t="s">
@@ -8201,7 +8212,7 @@
       </c>
     </row>
     <row r="329" spans="1:3" ht="52" x14ac:dyDescent="0.15">
-      <c r="A329" s="3" t="s">
+      <c r="A329" s="5" t="s">
         <v>952</v>
       </c>
       <c r="B329" s="3" t="s">
@@ -8212,7 +8223,7 @@
       </c>
     </row>
     <row r="330" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A330" s="3" t="s">
+      <c r="A330" s="5" t="s">
         <v>955</v>
       </c>
       <c r="B330" s="3" t="s">
@@ -8223,7 +8234,7 @@
       </c>
     </row>
     <row r="331" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A331" s="3" t="s">
+      <c r="A331" s="5" t="s">
         <v>958</v>
       </c>
       <c r="B331" s="3" t="s">
@@ -8234,7 +8245,7 @@
       </c>
     </row>
     <row r="332" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A332" s="3" t="s">
+      <c r="A332" s="5" t="s">
         <v>961</v>
       </c>
       <c r="B332" s="3" t="s">
@@ -8245,7 +8256,7 @@
       </c>
     </row>
     <row r="333" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A333" s="3" t="s">
+      <c r="A333" s="5" t="s">
         <v>963</v>
       </c>
       <c r="B333" s="3" t="s">
@@ -8255,8 +8266,8 @@
         <v>965</v>
       </c>
     </row>
-    <row r="334" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A334" s="3" t="s">
+    <row r="334" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A334" s="5" t="s">
         <v>966</v>
       </c>
       <c r="B334" s="3" t="s">
@@ -8267,7 +8278,7 @@
       </c>
     </row>
     <row r="335" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A335" s="3" t="s">
+      <c r="A335" s="5" t="s">
         <v>968</v>
       </c>
       <c r="B335" s="3" t="s">
@@ -8278,7 +8289,7 @@
       </c>
     </row>
     <row r="336" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A336" s="3" t="s">
+      <c r="A336" s="5" t="s">
         <v>971</v>
       </c>
       <c r="B336" s="3" t="s">
@@ -8289,7 +8300,7 @@
       </c>
     </row>
     <row r="337" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A337" s="3" t="s">
+      <c r="A337" s="5" t="s">
         <v>973</v>
       </c>
       <c r="B337" s="3" t="s">
@@ -8300,7 +8311,7 @@
       </c>
     </row>
     <row r="338" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A338" s="3" t="s">
+      <c r="A338" s="5" t="s">
         <v>976</v>
       </c>
       <c r="B338" s="3" t="s">
@@ -8311,7 +8322,7 @@
       </c>
     </row>
     <row r="339" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A339" s="3" t="s">
+      <c r="A339" s="5" t="s">
         <v>979</v>
       </c>
       <c r="B339" s="3" t="s">
@@ -8322,7 +8333,7 @@
       </c>
     </row>
     <row r="340" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A340" s="3" t="s">
+      <c r="A340" s="5" t="s">
         <v>982</v>
       </c>
       <c r="B340" s="3" t="s">
@@ -8333,7 +8344,7 @@
       </c>
     </row>
     <row r="341" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A341" s="3" t="s">
+      <c r="A341" s="5" t="s">
         <v>985</v>
       </c>
       <c r="B341" s="3" t="s">
@@ -8344,7 +8355,7 @@
       </c>
     </row>
     <row r="342" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A342" s="3" t="s">
+      <c r="A342" s="5" t="s">
         <v>988</v>
       </c>
       <c r="B342" s="3" t="s">
@@ -8355,7 +8366,7 @@
       </c>
     </row>
     <row r="343" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A343" s="3" t="s">
+      <c r="A343" s="5" t="s">
         <v>991</v>
       </c>
       <c r="B343" s="3" t="s">
@@ -8366,7 +8377,7 @@
       </c>
     </row>
     <row r="344" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A344" s="3" t="s">
+      <c r="A344" s="5" t="s">
         <v>994</v>
       </c>
       <c r="B344" s="3" t="s">
@@ -8377,7 +8388,7 @@
       </c>
     </row>
     <row r="345" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A345" s="3" t="s">
+      <c r="A345" s="5" t="s">
         <v>997</v>
       </c>
       <c r="B345" s="3" t="s">
@@ -8388,7 +8399,7 @@
       </c>
     </row>
     <row r="346" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A346" s="3" t="s">
+      <c r="A346" s="5" t="s">
         <v>1000</v>
       </c>
       <c r="B346" s="3" t="s">
@@ -8399,7 +8410,7 @@
       </c>
     </row>
     <row r="347" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A347" s="3" t="s">
+      <c r="A347" s="5" t="s">
         <v>1003</v>
       </c>
       <c r="B347" s="3" t="s">
@@ -8410,7 +8421,7 @@
       </c>
     </row>
     <row r="348" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A348" s="3" t="s">
+      <c r="A348" s="5" t="s">
         <v>1004</v>
       </c>
       <c r="B348" s="3" t="s">
@@ -8421,7 +8432,7 @@
       </c>
     </row>
     <row r="349" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A349" s="3" t="s">
+      <c r="A349" s="5" t="s">
         <v>1006</v>
       </c>
       <c r="B349" s="3" t="s">
@@ -8432,7 +8443,7 @@
       </c>
     </row>
     <row r="350" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A350" s="3" t="s">
+      <c r="A350" s="5" t="s">
         <v>1008</v>
       </c>
       <c r="B350" s="3" t="s">
@@ -8443,7 +8454,7 @@
       </c>
     </row>
     <row r="351" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A351" s="3" t="s">
+      <c r="A351" s="5" t="s">
         <v>1011</v>
       </c>
       <c r="B351" s="3" t="s">
@@ -8454,7 +8465,7 @@
       </c>
     </row>
     <row r="352" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A352" s="3" t="s">
+      <c r="A352" s="5" t="s">
         <v>1014</v>
       </c>
       <c r="B352" s="3" t="s">
@@ -8465,7 +8476,7 @@
       </c>
     </row>
     <row r="353" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A353" s="3" t="s">
+      <c r="A353" s="5" t="s">
         <v>1016</v>
       </c>
       <c r="B353" s="3" t="s">
@@ -8476,7 +8487,7 @@
       </c>
     </row>
     <row r="354" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A354" s="3" t="s">
+      <c r="A354" s="5" t="s">
         <v>1019</v>
       </c>
       <c r="B354" s="3" t="s">
@@ -8487,7 +8498,7 @@
       </c>
     </row>
     <row r="355" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A355" s="3" t="s">
+      <c r="A355" s="5" t="s">
         <v>1022</v>
       </c>
       <c r="B355" s="3" t="s">
@@ -8498,7 +8509,7 @@
       </c>
     </row>
     <row r="356" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A356" s="3" t="s">
+      <c r="A356" s="5" t="s">
         <v>1025</v>
       </c>
       <c r="B356" s="3" t="s">
@@ -8509,7 +8520,7 @@
       </c>
     </row>
     <row r="357" spans="1:3" ht="78" x14ac:dyDescent="0.15">
-      <c r="A357" s="3" t="s">
+      <c r="A357" s="5" t="s">
         <v>1028</v>
       </c>
       <c r="B357" s="3" t="s">
@@ -8520,7 +8531,7 @@
       </c>
     </row>
     <row r="358" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A358" s="3" t="s">
+      <c r="A358" s="5" t="s">
         <v>1031</v>
       </c>
       <c r="B358" s="3" t="s">
@@ -8531,7 +8542,7 @@
       </c>
     </row>
     <row r="359" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A359" s="3" t="s">
+      <c r="A359" s="5" t="s">
         <v>1034</v>
       </c>
       <c r="B359" s="3" t="s">
@@ -8542,7 +8553,7 @@
       </c>
     </row>
     <row r="360" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A360" s="3" t="s">
+      <c r="A360" s="5" t="s">
         <v>1037</v>
       </c>
       <c r="B360" s="3" t="s">
@@ -8553,7 +8564,7 @@
       </c>
     </row>
     <row r="361" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A361" s="3" t="s">
+      <c r="A361" s="5" t="s">
         <v>1039</v>
       </c>
       <c r="B361" s="3" t="s">
@@ -8564,7 +8575,7 @@
       </c>
     </row>
     <row r="362" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A362" s="3" t="s">
+      <c r="A362" s="5" t="s">
         <v>1042</v>
       </c>
       <c r="B362" s="3" t="s">
@@ -8575,7 +8586,7 @@
       </c>
     </row>
     <row r="363" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A363" s="3" t="s">
+      <c r="A363" s="5" t="s">
         <v>1045</v>
       </c>
       <c r="B363" s="3" t="s">
@@ -8586,7 +8597,7 @@
       </c>
     </row>
     <row r="364" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A364" s="3" t="s">
+      <c r="A364" s="5" t="s">
         <v>1048</v>
       </c>
       <c r="B364" s="3" t="s">
@@ -8597,7 +8608,7 @@
       </c>
     </row>
     <row r="365" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A365" s="3" t="s">
+      <c r="A365" s="5" t="s">
         <v>1050</v>
       </c>
       <c r="B365" s="3" t="s">
@@ -8608,7 +8619,7 @@
       </c>
     </row>
     <row r="366" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A366" s="3" t="s">
+      <c r="A366" s="5" t="s">
         <v>1052</v>
       </c>
       <c r="B366" s="3" t="s">
@@ -8619,7 +8630,7 @@
       </c>
     </row>
     <row r="367" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A367" s="3" t="s">
+      <c r="A367" s="5" t="s">
         <v>1055</v>
       </c>
       <c r="B367" s="3" t="s">
@@ -8630,7 +8641,7 @@
       </c>
     </row>
     <row r="368" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A368" s="3" t="s">
+      <c r="A368" s="5" t="s">
         <v>1058</v>
       </c>
       <c r="B368" s="3" t="s">
@@ -8641,7 +8652,7 @@
       </c>
     </row>
     <row r="369" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A369" s="3" t="s">
+      <c r="A369" s="5" t="s">
         <v>1060</v>
       </c>
       <c r="B369" s="3" t="s">
@@ -8652,7 +8663,7 @@
       </c>
     </row>
     <row r="370" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A370" s="3" t="s">
+      <c r="A370" s="5" t="s">
         <v>1063</v>
       </c>
       <c r="B370" s="3" t="s">
@@ -8663,7 +8674,7 @@
       </c>
     </row>
     <row r="371" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A371" s="3" t="s">
+      <c r="A371" s="5" t="s">
         <v>1066</v>
       </c>
       <c r="B371" s="3" t="s">
@@ -8674,7 +8685,7 @@
       </c>
     </row>
     <row r="372" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A372" s="3" t="s">
+      <c r="A372" s="5" t="s">
         <v>1069</v>
       </c>
       <c r="B372" s="3" t="s">
@@ -8685,7 +8696,7 @@
       </c>
     </row>
     <row r="373" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A373" s="3" t="s">
+      <c r="A373" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="B373" s="3" t="s">
@@ -8696,7 +8707,7 @@
       </c>
     </row>
     <row r="374" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A374" s="3" t="s">
+      <c r="A374" s="5" t="s">
         <v>1075</v>
       </c>
       <c r="B374" s="3" t="s">
@@ -8707,7 +8718,7 @@
       </c>
     </row>
     <row r="375" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A375" s="3" t="s">
+      <c r="A375" s="5" t="s">
         <v>1078</v>
       </c>
       <c r="B375" s="3" t="s">
@@ -8718,7 +8729,7 @@
       </c>
     </row>
     <row r="376" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A376" s="3" t="s">
+      <c r="A376" s="5" t="s">
         <v>1081</v>
       </c>
       <c r="B376" s="3" t="s">
@@ -8729,7 +8740,7 @@
       </c>
     </row>
     <row r="377" spans="1:3" ht="91" x14ac:dyDescent="0.15">
-      <c r="A377" s="3" t="s">
+      <c r="A377" s="5" t="s">
         <v>1084</v>
       </c>
       <c r="B377" s="3" t="s">
@@ -8740,7 +8751,7 @@
       </c>
     </row>
     <row r="378" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A378" s="3" t="s">
+      <c r="A378" s="5" t="s">
         <v>1087</v>
       </c>
       <c r="B378" s="3" t="s">
@@ -8751,7 +8762,7 @@
       </c>
     </row>
     <row r="379" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A379" s="3" t="s">
+      <c r="A379" s="5" t="s">
         <v>1090</v>
       </c>
       <c r="B379" s="3" t="s">
@@ -8762,7 +8773,7 @@
       </c>
     </row>
     <row r="380" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A380" s="3" t="s">
+      <c r="A380" s="5" t="s">
         <v>1093</v>
       </c>
       <c r="B380" s="3" t="s">
@@ -8773,7 +8784,7 @@
       </c>
     </row>
     <row r="381" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A381" s="3" t="s">
+      <c r="A381" s="5" t="s">
         <v>1096</v>
       </c>
       <c r="B381" s="3" t="s">
@@ -8784,7 +8795,7 @@
       </c>
     </row>
     <row r="382" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A382" s="3" t="s">
+      <c r="A382" s="5" t="s">
         <v>1099</v>
       </c>
       <c r="B382" s="3" t="s">
@@ -8795,7 +8806,7 @@
       </c>
     </row>
     <row r="383" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A383" s="3" t="s">
+      <c r="A383" s="5" t="s">
         <v>1102</v>
       </c>
       <c r="B383" s="3" t="s">
@@ -8806,7 +8817,7 @@
       </c>
     </row>
     <row r="384" spans="1:3" ht="52" x14ac:dyDescent="0.15">
-      <c r="A384" s="3" t="s">
+      <c r="A384" s="5" t="s">
         <v>1105</v>
       </c>
       <c r="B384" s="3" t="s">
@@ -8817,7 +8828,7 @@
       </c>
     </row>
     <row r="385" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A385" s="3" t="s">
+      <c r="A385" s="5" t="s">
         <v>1108</v>
       </c>
       <c r="B385" s="3" t="s">
@@ -8828,7 +8839,7 @@
       </c>
     </row>
     <row r="386" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A386" s="3" t="s">
+      <c r="A386" s="5" t="s">
         <v>1111</v>
       </c>
       <c r="B386" s="3" t="s">
@@ -8839,7 +8850,7 @@
       </c>
     </row>
     <row r="387" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A387" s="3" t="s">
+      <c r="A387" s="5" t="s">
         <v>1114</v>
       </c>
       <c r="B387" s="3" t="s">
@@ -8850,7 +8861,7 @@
       </c>
     </row>
     <row r="388" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A388" s="3" t="s">
+      <c r="A388" s="5" t="s">
         <v>1117</v>
       </c>
       <c r="B388" s="3" t="s">
@@ -8860,8 +8871,8 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="389" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A389" s="3" t="s">
+    <row r="389" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A389" s="5" t="s">
         <v>1120</v>
       </c>
       <c r="B389" s="3" t="s">
@@ -8872,7 +8883,7 @@
       </c>
     </row>
     <row r="390" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A390" s="3" t="s">
+      <c r="A390" s="5" t="s">
         <v>1123</v>
       </c>
       <c r="B390" s="3" t="s">
@@ -8883,7 +8894,7 @@
       </c>
     </row>
     <row r="391" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A391" s="3" t="s">
+      <c r="A391" s="5" t="s">
         <v>1126</v>
       </c>
       <c r="B391" s="3" t="s">
@@ -8894,7 +8905,7 @@
       </c>
     </row>
     <row r="392" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A392" s="3" t="s">
+      <c r="A392" s="5" t="s">
         <v>1129</v>
       </c>
       <c r="B392" s="3" t="s">
@@ -8905,7 +8916,7 @@
       </c>
     </row>
     <row r="393" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A393" s="3" t="s">
+      <c r="A393" s="5" t="s">
         <v>1132</v>
       </c>
       <c r="B393" s="3" t="s">
@@ -8916,7 +8927,7 @@
       </c>
     </row>
     <row r="394" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A394" s="3" t="s">
+      <c r="A394" s="5" t="s">
         <v>1134</v>
       </c>
       <c r="B394" s="3" t="s">
@@ -8927,7 +8938,7 @@
       </c>
     </row>
     <row r="395" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A395" s="3" t="s">
+      <c r="A395" s="5" t="s">
         <v>1137</v>
       </c>
       <c r="B395" s="3" t="s">
@@ -8938,7 +8949,7 @@
       </c>
     </row>
     <row r="396" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A396" s="3" t="s">
+      <c r="A396" s="5" t="s">
         <v>1139</v>
       </c>
       <c r="B396" s="3" t="s">
@@ -8949,7 +8960,7 @@
       </c>
     </row>
     <row r="397" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A397" s="3" t="s">
+      <c r="A397" s="5" t="s">
         <v>1142</v>
       </c>
       <c r="B397" s="3" t="s">
@@ -8960,7 +8971,7 @@
       </c>
     </row>
     <row r="398" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A398" s="3" t="s">
+      <c r="A398" s="5" t="s">
         <v>1145</v>
       </c>
       <c r="B398" s="3" t="s">
@@ -8971,7 +8982,7 @@
       </c>
     </row>
     <row r="399" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A399" s="3" t="s">
+      <c r="A399" s="5" t="s">
         <v>1148</v>
       </c>
       <c r="B399" s="3" t="s">
@@ -8982,7 +8993,7 @@
       </c>
     </row>
     <row r="400" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A400" s="3" t="s">
+      <c r="A400" s="5" t="s">
         <v>1149</v>
       </c>
       <c r="B400" s="3" t="s">
@@ -8993,7 +9004,7 @@
       </c>
     </row>
     <row r="401" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A401" s="3" t="s">
+      <c r="A401" s="5" t="s">
         <v>1151</v>
       </c>
       <c r="B401" s="3" t="s">
@@ -9004,7 +9015,7 @@
       </c>
     </row>
     <row r="402" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A402" s="3" t="s">
+      <c r="A402" s="5" t="s">
         <v>1154</v>
       </c>
       <c r="B402" s="3" t="s">
@@ -9015,7 +9026,7 @@
       </c>
     </row>
     <row r="403" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A403" s="3" t="s">
+      <c r="A403" s="5" t="s">
         <v>1157</v>
       </c>
       <c r="B403" s="3" t="s">
@@ -9026,7 +9037,7 @@
       </c>
     </row>
     <row r="404" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A404" s="3" t="s">
+      <c r="A404" s="5" t="s">
         <v>1160</v>
       </c>
       <c r="B404" s="3" t="s">
@@ -9037,7 +9048,7 @@
       </c>
     </row>
     <row r="405" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A405" s="3" t="s">
+      <c r="A405" s="5" t="s">
         <v>1163</v>
       </c>
       <c r="B405" s="3" t="s">
@@ -9048,7 +9059,7 @@
       </c>
     </row>
     <row r="406" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A406" s="3" t="s">
+      <c r="A406" s="5" t="s">
         <v>1166</v>
       </c>
       <c r="B406" s="3" t="s">
@@ -9059,7 +9070,7 @@
       </c>
     </row>
     <row r="407" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A407" s="3" t="s">
+      <c r="A407" s="5" t="s">
         <v>1169</v>
       </c>
       <c r="B407" s="3" t="s">
@@ -9070,7 +9081,7 @@
       </c>
     </row>
     <row r="408" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A408" s="3" t="s">
+      <c r="A408" s="5" t="s">
         <v>1172</v>
       </c>
       <c r="B408" s="3" t="s">
@@ -9081,7 +9092,7 @@
       </c>
     </row>
     <row r="409" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A409" s="3" t="s">
+      <c r="A409" s="5" t="s">
         <v>1175</v>
       </c>
       <c r="B409" s="3" t="s">
@@ -9092,7 +9103,7 @@
       </c>
     </row>
     <row r="410" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A410" s="3" t="s">
+      <c r="A410" s="5" t="s">
         <v>1178</v>
       </c>
       <c r="B410" s="3" t="s">
@@ -9103,7 +9114,7 @@
       </c>
     </row>
     <row r="411" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A411" s="3" t="s">
+      <c r="A411" s="5" t="s">
         <v>1179</v>
       </c>
       <c r="B411" s="3" t="s">
@@ -9114,7 +9125,7 @@
       </c>
     </row>
     <row r="412" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A412" s="3" t="s">
+      <c r="A412" s="5" t="s">
         <v>1181</v>
       </c>
       <c r="B412" s="3" t="s">
@@ -9125,7 +9136,7 @@
       </c>
     </row>
     <row r="413" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A413" s="3" t="s">
+      <c r="A413" s="5" t="s">
         <v>1184</v>
       </c>
       <c r="B413" s="3" t="s">
@@ -9136,7 +9147,7 @@
       </c>
     </row>
     <row r="414" spans="1:3" ht="39" x14ac:dyDescent="0.15">
-      <c r="A414" s="3" t="s">
+      <c r="A414" s="5" t="s">
         <v>1187</v>
       </c>
       <c r="B414" s="3" t="s">
@@ -9147,7 +9158,7 @@
       </c>
     </row>
     <row r="415" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A415" s="3" t="s">
+      <c r="A415" s="5" t="s">
         <v>1190</v>
       </c>
       <c r="B415" s="3" t="s">
@@ -9158,7 +9169,7 @@
       </c>
     </row>
     <row r="416" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A416" s="3" t="s">
+      <c r="A416" s="5" t="s">
         <v>1193</v>
       </c>
       <c r="B416" s="3" t="s">
@@ -9169,7 +9180,7 @@
       </c>
     </row>
     <row r="417" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A417" s="3" t="s">
+      <c r="A417" s="5" t="s">
         <v>1196</v>
       </c>
       <c r="B417" s="3" t="s">
@@ -9180,7 +9191,7 @@
       </c>
     </row>
     <row r="418" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A418" s="3" t="s">
+      <c r="A418" s="5" t="s">
         <v>1199</v>
       </c>
       <c r="B418" s="3" t="s">
@@ -9191,7 +9202,7 @@
       </c>
     </row>
     <row r="419" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A419" s="3" t="s">
+      <c r="A419" s="5" t="s">
         <v>1202</v>
       </c>
       <c r="B419" s="3" t="s">
@@ -9202,7 +9213,7 @@
       </c>
     </row>
     <row r="420" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A420" s="3" t="s">
+      <c r="A420" s="5" t="s">
         <v>1205</v>
       </c>
       <c r="B420" s="3" t="s">
@@ -9213,7 +9224,7 @@
       </c>
     </row>
     <row r="421" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A421" s="3" t="s">
+      <c r="A421" s="5" t="s">
         <v>1208</v>
       </c>
       <c r="B421" s="3" t="s">
@@ -9224,7 +9235,7 @@
       </c>
     </row>
     <row r="422" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A422" s="3" t="s">
+      <c r="A422" s="5" t="s">
         <v>1210</v>
       </c>
       <c r="B422" s="3" t="s">
@@ -9235,7 +9246,7 @@
       </c>
     </row>
     <row r="423" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A423" s="3" t="s">
+      <c r="A423" s="5" t="s">
         <v>1212</v>
       </c>
       <c r="B423" s="3" t="s">
@@ -9246,7 +9257,7 @@
       </c>
     </row>
     <row r="424" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A424" s="3" t="s">
+      <c r="A424" s="5" t="s">
         <v>1215</v>
       </c>
       <c r="B424" s="3" t="s">
@@ -9257,7 +9268,7 @@
       </c>
     </row>
     <row r="425" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A425" s="3" t="s">
+      <c r="A425" s="5" t="s">
         <v>1217</v>
       </c>
       <c r="B425" s="3" t="s">
@@ -9267,8 +9278,8 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="426" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A426" s="3" t="s">
+    <row r="426" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A426" s="5" t="s">
         <v>1220</v>
       </c>
       <c r="B426" s="3" t="s">
@@ -9279,7 +9290,7 @@
       </c>
     </row>
     <row r="427" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A427" s="3" t="s">
+      <c r="A427" s="5" t="s">
         <v>1223</v>
       </c>
       <c r="B427" s="3" t="s">

</xml_diff>